<commit_message>
Updating Test Case file
</commit_message>
<xml_diff>
--- a/src/test/java/com/practo/PractoCW_Test.xlsx
+++ b/src/test/java/com/practo/PractoCW_Test.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cognizant\JavaPractice\Hackathon_FindingHospitals\src\test\java\com\practo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cognizant\JavaPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09494D00-4478-4A42-811E-7577D33D7B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E115C90-130A-4B49-A7BE-3857A70BC844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -413,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,6 +489,222 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="sharman@" xr:uid="{2345182A-31BE-4038-931F-238D5B9FAAC6}"/>
@@ -497,235 +712,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05DAA8CF-0F64-462E-AC23-4E433ECB785D}">
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
-        <v>3</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>20</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>